<commit_message>
added programs based on the pass by reference
</commit_message>
<xml_diff>
--- a/LAB/Copy of course_plan_-_C_Lab(1).xlsx
+++ b/LAB/Copy of course_plan_-_C_Lab(1).xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added 2d array and pointers programs
</commit_message>
<xml_diff>
--- a/LAB/Copy of course_plan_-_C_Lab(1).xlsx
+++ b/LAB/Copy of course_plan_-_C_Lab(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71a259dc963d91c3/Desktop/GPTC/S3-PROGRAMMING_IN_C/LAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC9857DB-64D0-48CF-8D0E-10B899E334E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{EC9857DB-64D0-48CF-8D0E-10B899E334E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E009678-3CC8-4EC9-98C0-67E2FAE069EE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,6 +529,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,7 +736,7 @@
   <dimension ref="A1:J224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>